<commit_message>
Add findFilterBySearch for CDS facet dropdown for PHS Accession filtering
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC02_CDS_phs001819_SampleTumorStatus-NSD_SampleType-BloodDerivedNormal.xlsx
+++ b/InputFiles/CDS/TC02_CDS_phs001819_SampleTumorStatus-NSD_SampleType-BloodDerivedNormal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/CDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58416B9-FC16-1B4B-B5D6-DDABDF598219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AADA3B4-C060-7D4A-BD0D-7813B9D6388A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -258,9 +258,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -313,14 +320,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -643,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -676,7 +686,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -715,7 +725,7 @@
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>